<commit_message>
Updated Project Status XLS
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="34">
   <si>
     <t>Status:</t>
   </si>
@@ -535,7 +535,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +554,7 @@
       <c r="C1" s="9"/>
       <c r="D1" s="2">
         <f ca="1">TODAY()</f>
-        <v>44669</v>
+        <v>44670</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -647,7 +647,9 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="7" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
Added Sega Genesis/Megadrive Multitap Support
Added PCB/Gerber and Update SW CAD/ Added STLs for the Genesis/Megadrive Multitap version.
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="37">
   <si>
     <t>Status:</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>PS2</t>
+  </si>
+  <si>
+    <t>Genesis - Multitap</t>
+  </si>
+  <si>
+    <t>Megadrive - Multitap</t>
+  </si>
+  <si>
+    <t>Megadrive</t>
   </si>
 </sst>
 </file>
@@ -532,10 +541,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +563,7 @@
       <c r="C1" s="9"/>
       <c r="D1" s="2">
         <f ca="1">TODAY()</f>
-        <v>44670</v>
+        <v>44671</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -735,7 +744,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>17</v>
@@ -747,7 +756,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>17</v>
@@ -759,7 +768,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>17</v>
@@ -771,7 +780,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>17</v>
@@ -783,7 +792,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>17</v>
@@ -791,13 +800,11 @@
       <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>17</v>
@@ -809,7 +816,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>17</v>
@@ -821,7 +828,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>17</v>
@@ -835,7 +842,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>17</v>
@@ -843,13 +850,11 @@
       <c r="C24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>17</v>
@@ -861,15 +866,21 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+        <v>33</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>17</v>
@@ -877,11 +888,13 @@
       <c r="C27" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>17</v>
@@ -889,33 +902,65 @@
       <c r="C28" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>17</v>
-      </c>
+      <c r="D28" s="7"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>17</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="7" t="s">
+      <c r="B33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates from Issues 42/43/18
Closed Issues 42 and 43 as Sega Genesis and PSX have been successfully tested and functional.

Updated Dreamcast PCB per comment in Issue 18 - Reversed P1-P4 pads to match housing

Updated Project Status to reflect #42 and #43 Complete
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17832"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
   <si>
     <t>Status:</t>
   </si>
@@ -544,18 +544,18 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D33" sqref="A1:D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="5"/>
+    <col min="2" max="3" width="24.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -563,10 +563,10 @@
       <c r="C1" s="9"/>
       <c r="D1" s="2">
         <f ca="1">TODAY()</f>
-        <v>44726</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+        <v>44815</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -580,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -592,7 +592,7 @@
       </c>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -604,7 +604,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -616,7 +616,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -628,7 +628,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -640,7 +640,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -652,7 +652,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -664,7 +664,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -676,7 +676,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -690,7 +690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -702,7 +702,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -716,7 +716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -730,7 +730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -740,9 +740,11 @@
       <c r="C15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="7"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -752,9 +754,11 @@
       <c r="C16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="7"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D16" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -764,9 +768,11 @@
       <c r="C17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -776,9 +782,11 @@
       <c r="C18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -790,7 +798,7 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -802,7 +810,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -814,7 +822,7 @@
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -826,7 +834,7 @@
       </c>
       <c r="D22" s="7"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -840,7 +848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -852,7 +860,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -862,9 +870,11 @@
       <c r="C25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D25" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -878,7 +888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -892,7 +902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -906,7 +916,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
@@ -914,7 +924,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
@@ -926,7 +936,7 @@
       </c>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -940,7 +950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -952,7 +962,7 @@
       </c>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Wii Ext, NES/SNES mini PCB design complete (#59)
* PCB Design

Started design of Wii Ext & NES/SNES Mini PCBs

I ordered the initial PCB and will update once I receive them

Once the PCB is verified, I will work on the housing CAD

* Adding USB-C Datasheet and Library

* Update README.md

* Update BOM.xlsx

Added info for Wii Ext & SNES/NES Mini PCB components

* Retiring Main PCB

Retiring Original Main PCB design as the unit is thinner that the standard footprint.  This was causing  confusion.  The new main used to be Main Alt Wide version.  It is now the standard as it fits the standard ESP footprint.  The Thinner version has been moved to the retired folder in PCBs

* Adding FW 1.7.3 from Darthcloud

* Wii Ext, NES/SNES Mini PCB Design Status

Design is complete, updating BOM and project Status before merging.
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="41">
   <si>
     <t>Status:</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>Megadrive</t>
+  </si>
+  <si>
+    <t>Wii Ext</t>
+  </si>
+  <si>
+    <t>NES Mini</t>
+  </si>
+  <si>
+    <t>SNES Mini</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -190,7 +202,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -237,11 +249,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -258,6 +283,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,29 +567,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="A1:D33"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="2">
         <f ca="1">TODAY()</f>
-        <v>44815</v>
+        <v>44893</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -796,7 +820,9 @@
       <c r="C19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -808,7 +834,9 @@
       <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -820,7 +848,9 @@
       <c r="C21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -960,7 +990,9 @@
       <c r="C32" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="D32" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
@@ -976,8 +1008,50 @@
         <v>17</v>
       </c>
     </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="77" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wii ext nes snes classic cad (#62)
* CAD Update

I have completed the preliminary CAD for the Wii EXT & NES/SNES Classic PCBs.  I have ordered them from Shapeways and will merge the branch if no additional changes are needed.

Included in this commit are the following:
Updated CAD and STLs for the AUX housing Top for the NES Classic, SNES Classic, Famicom Classic, Super Famicom Classic, Wii Ext and Oprional Wii

The Aux Bottom that covers all the variants mentioned above.

As Always the CAD is included and the new font for the Wii Variants is included as well.

* Updated Housing color for renders

* VB Housing and File House Keeping

Created the housing for the Virtual Boy, added a 3D printable VB controller plug parts (Thanks RetroOnyx)

Renamed all STLs with Console Company Names for consistency

Updated the BOM for the Virtual Boy Parts and Added 3D Printed Parts for BOM also.

* Updated Project Status

Marking the new PCB and housing design complete
</commit_message>
<xml_diff>
--- a/Project Status.xlsx
+++ b/Project Status.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$36</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="40">
   <si>
     <t>Status:</t>
   </si>
@@ -144,9 +147,6 @@
   </si>
   <si>
     <t>SNES Mini</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -569,17 +569,19 @@
   </sheetPr>
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="5"/>
+    <col min="2" max="3" width="24.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.65">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -587,10 +589,10 @@
       <c r="C1" s="9"/>
       <c r="D1" s="2">
         <f ca="1">TODAY()</f>
-        <v>44893</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+        <v>44929</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -604,7 +606,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -614,9 +616,11 @@
       <c r="C3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -626,9 +630,11 @@
       <c r="C4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -640,7 +646,7 @@
       </c>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>21</v>
       </c>
@@ -652,7 +658,7 @@
       </c>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -664,7 +670,7 @@
       </c>
       <c r="D7" s="7"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -676,7 +682,7 @@
       </c>
       <c r="D8" s="7"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -688,7 +694,7 @@
       </c>
       <c r="D9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -700,7 +706,7 @@
       </c>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -714,7 +720,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -726,7 +732,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -740,7 +746,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -754,7 +760,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -768,7 +774,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -782,7 +788,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -796,7 +802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
@@ -810,7 +816,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -824,7 +830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -838,7 +844,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -852,7 +858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -862,9 +868,11 @@
       <c r="C22" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -878,7 +886,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -890,7 +898,7 @@
       </c>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
@@ -904,7 +912,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -918,7 +926,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -932,7 +940,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>10</v>
       </c>
@@ -946,7 +954,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
@@ -954,7 +962,7 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
@@ -966,7 +974,7 @@
       </c>
       <c r="D30" s="7"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -980,7 +988,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -994,7 +1002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1008,7 +1016,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -1016,13 +1024,13 @@
         <v>17</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>38</v>
       </c>
@@ -1030,13 +1038,13 @@
         <v>17</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>39</v>
       </c>
@@ -1044,7 +1052,7 @@
         <v>17</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>17</v>
@@ -1052,6 +1060,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="91" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>